<commit_message>
almost finished loading diagram
</commit_message>
<xml_diff>
--- a/aircraftTLARspecifications2024.xlsx
+++ b/aircraftTLARspecifications2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Aerospace\ADSEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5F6D7F-E9A7-4A86-B899-FEECE29BDAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7657F43-9E25-453A-857D-FB6ACE6FD1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,9 +511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG501"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG37" activeCellId="1" sqref="AG1 AG37"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -51165,7 +51165,7 @@
   <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>